<commit_message>
feat: add summary table
</commit_message>
<xml_diff>
--- a/海峡两岸汉字对照表附注.xlsx
+++ b/海峡两岸汉字对照表附注.xlsx
@@ -1472,9 +1472,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -1515,8 +1515,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1529,8 +1544,40 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1546,62 +1593,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1615,22 +1607,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1657,7 +1657,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1669,13 +1681,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1687,7 +1741,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1699,25 +1771,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1729,103 +1819,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1857,6 +1857,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1868,45 +1877,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1936,6 +1906,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1944,82 +1944,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2031,50 +2031,50 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -16196,8 +16196,8 @@
   <sheetPr/>
   <dimension ref="A1:AU167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:E56"/>
+    <sheetView tabSelected="1" topLeftCell="K104" workbookViewId="0">
+      <selection activeCell="S118" sqref="S118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -23501,7 +23501,7 @@
       </c>
       <c r="R118" s="1"/>
       <c r="S118" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="T118" s="1" t="s">
         <v>8</v>

</xml_diff>